<commit_message>
cambios en el reporte
</commit_message>
<xml_diff>
--- a/reports/inscritos.xlsx
+++ b/reports/inscritos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
   <si>
     <t>PARTICIPANTE</t>
   </si>
@@ -31,6 +31,9 @@
     <t>TIPO DE INSCRIPCIÓN</t>
   </si>
   <si>
+    <t>INSTITUCIÓN</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ramírez Buendía Daniel Sebastián </t>
   </si>
   <si>
@@ -49,10 +52,76 @@
     <t>Autores - Primer Artículo</t>
   </si>
   <si>
+    <t>ESPE</t>
+  </si>
+  <si>
     <t>Profesionales y Profesores Externos</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>Estudiante EPN Pregrado</t>
+  </si>
+  <si>
+    <t>Escuela Politécnica Nacional</t>
+  </si>
+  <si>
+    <t>Chasiloa Páez Mirian Amparo</t>
+  </si>
+  <si>
+    <t>1709691495</t>
+  </si>
+  <si>
+    <t>jennymq44@hotmail.com</t>
+  </si>
+  <si>
+    <t>+593 0998179204</t>
+  </si>
+  <si>
+    <t>Calderón</t>
+  </si>
+  <si>
+    <t>Estudiante EPN Postgrado</t>
+  </si>
+  <si>
+    <t>EPN</t>
+  </si>
+  <si>
+    <t>Quiguango Rivera Alisson Lorena</t>
+  </si>
+  <si>
+    <t>1003834627</t>
+  </si>
+  <si>
+    <t>jennymq44@gmail.com</t>
+  </si>
+  <si>
+    <t>+593 0338138035</t>
+  </si>
+  <si>
+    <t>PUCE</t>
+  </si>
+  <si>
+    <t>Buendía Ramírez Sebastián Daniel</t>
+  </si>
+  <si>
+    <t>danielsanramirez@hotmail.com</t>
+  </si>
+  <si>
+    <t>La Florida</t>
+  </si>
+  <si>
+    <t>UDLA</t>
+  </si>
+  <si>
+    <t>Ramírez Daniel</t>
+  </si>
+  <si>
+    <t>dsramirez1193@gmail.com</t>
+  </si>
+  <si>
+    <t>+297 4846518</t>
   </si>
 </sst>
 </file>
@@ -429,17 +498,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
     <col min="4" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="50" customWidth="1"/>
+    <col min="6" max="7" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,65 +527,215 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
-        <v>13</v>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>